<commit_message>
Error graph and calibration
</commit_message>
<xml_diff>
--- a/DistanceCalibrationData.xlsx
+++ b/DistanceCalibrationData.xlsx
@@ -13,6 +13,20 @@
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Sensor output</t>
+  </si>
+  <si>
+    <t>Object Distance (cm)</t>
+  </si>
+  <si>
+    <t>Test of points not used for calibration</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -60,6 +74,209 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sensor output</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$4:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="1">
+                  <c:v>494</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>294</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="48696320"/>
+        <c:axId val="118712000"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="48696320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="118712000"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="118712000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="48696320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>385762</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>80962</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -349,13 +566,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>30</v>
+      </c>
+      <c r="B6">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>40</v>
+      </c>
+      <c r="B7">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>50</v>
+      </c>
+      <c r="B8">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>60</v>
+      </c>
+      <c r="B9">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>70</v>
+      </c>
+      <c r="B10">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>80</v>
+      </c>
+      <c r="B11">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>25</v>
+      </c>
+      <c r="B19">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>35</v>
+      </c>
+      <c r="B20">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>45</v>
+      </c>
+      <c r="B21">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>55</v>
+      </c>
+      <c r="B22">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>65</v>
+      </c>
+      <c r="B23">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>75</v>
+      </c>
+      <c r="B24">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>